<commit_message>
added code to calculate squarness of non-constrained RHC
</commit_message>
<xml_diff>
--- a/how_sqaure_is_my_square.xlsx
+++ b/how_sqaure_is_my_square.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Q</t>
   </si>
@@ -55,13 +55,16 @@
   <si>
     <t>squarness alg failed, very bad</t>
   </si>
+  <si>
+    <t>RHC w/o constraints</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -189,7 +192,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T14"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1328,8 +1331,121 @@
         <v>9</v>
       </c>
     </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>10</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>50</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17">
+        <v>50</v>
+      </c>
+      <c r="H17" s="1">
+        <v>2</v>
+      </c>
+      <c r="I17" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="J17" s="14">
+        <v>5</v>
+      </c>
+      <c r="K17" s="14">
+        <v>5</v>
+      </c>
+      <c r="L17" s="14">
+        <v>30</v>
+      </c>
+      <c r="M17" s="1">
+        <v>30</v>
+      </c>
+      <c r="N17" s="13">
+        <v>30</v>
+      </c>
+      <c r="O17" s="13">
+        <v>10</v>
+      </c>
+      <c r="P17">
+        <v>20</v>
+      </c>
+      <c r="Q17">
+        <v>0.1</v>
+      </c>
+      <c r="R17" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="S17">
+        <v>0.1152</v>
+      </c>
+      <c r="T17" s="14"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="S3:S8 S15:S26">
+  <conditionalFormatting sqref="S3:S8 S15:S16 S18:S26">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S9">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S3:S9">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S10">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S10">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -1341,7 +1457,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S9">
+  <conditionalFormatting sqref="S3:S10">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -1353,7 +1469,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S9">
+  <conditionalFormatting sqref="S11">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -1365,7 +1481,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S10">
+  <conditionalFormatting sqref="S11">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -1377,7 +1493,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S10">
+  <conditionalFormatting sqref="S11">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -1389,7 +1505,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S10">
+  <conditionalFormatting sqref="S12">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -1401,7 +1517,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S11">
+  <conditionalFormatting sqref="S12">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -1413,7 +1529,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S11">
+  <conditionalFormatting sqref="S12">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -1425,7 +1541,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S11">
+  <conditionalFormatting sqref="S13">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -1437,7 +1553,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S12">
+  <conditionalFormatting sqref="S13">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -1449,7 +1565,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S12">
+  <conditionalFormatting sqref="S13">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -1461,7 +1577,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S12">
+  <conditionalFormatting sqref="S14">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -1473,7 +1589,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S13">
+  <conditionalFormatting sqref="S14">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -1485,7 +1601,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S13">
+  <conditionalFormatting sqref="S14">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -1497,56 +1613,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S13">
+  <conditionalFormatting sqref="S3:S14">
     <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S14">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S14">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S14">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S14">
-    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>

<commit_message>
added axis labels on figures, added figures and report
</commit_message>
<xml_diff>
--- a/how_sqaure_is_my_square.xlsx
+++ b/how_sqaure_is_my_square.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Q</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>RHC w/o constraints</t>
+  </si>
+  <si>
+    <t>best linear sim can handle</t>
   </si>
 </sst>
 </file>
@@ -507,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T17"/>
+  <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1396,8 +1399,121 @@
       </c>
       <c r="T17" s="14"/>
     </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>10</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>10</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>50</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <v>50</v>
+      </c>
+      <c r="H20" s="1">
+        <v>2</v>
+      </c>
+      <c r="I20" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="J20" s="14">
+        <v>5</v>
+      </c>
+      <c r="K20" s="14">
+        <v>5</v>
+      </c>
+      <c r="L20" s="14">
+        <v>30</v>
+      </c>
+      <c r="M20" s="1">
+        <v>30</v>
+      </c>
+      <c r="N20" s="13">
+        <v>30</v>
+      </c>
+      <c r="O20" s="13">
+        <v>10</v>
+      </c>
+      <c r="P20">
+        <v>20</v>
+      </c>
+      <c r="Q20">
+        <v>0.1</v>
+      </c>
+      <c r="R20" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="S20" s="15">
+        <v>2.87E-2</v>
+      </c>
+      <c r="T20" s="14"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="S3:S8 S15:S16 S18:S26">
+  <conditionalFormatting sqref="S3:S8 S15:S16 S18:S19 S21:S26">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S9">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S3:S9">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S10">
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S10">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -1409,7 +1525,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S9">
+  <conditionalFormatting sqref="S3:S10">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -1421,7 +1537,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S9">
+  <conditionalFormatting sqref="S11">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -1433,7 +1549,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S10">
+  <conditionalFormatting sqref="S11">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -1445,7 +1561,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S10">
+  <conditionalFormatting sqref="S11">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -1457,7 +1573,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S10">
+  <conditionalFormatting sqref="S12">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -1469,7 +1585,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S11">
+  <conditionalFormatting sqref="S12">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -1481,7 +1597,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S11">
+  <conditionalFormatting sqref="S12">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -1493,7 +1609,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S11">
+  <conditionalFormatting sqref="S13">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -1505,7 +1621,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S12">
+  <conditionalFormatting sqref="S13">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -1517,7 +1633,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S12">
+  <conditionalFormatting sqref="S13">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -1529,7 +1645,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S12">
+  <conditionalFormatting sqref="S14">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -1541,7 +1657,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S13">
+  <conditionalFormatting sqref="S14">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -1553,7 +1669,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S13">
+  <conditionalFormatting sqref="S14">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -1565,7 +1681,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S13">
+  <conditionalFormatting sqref="S3:S14">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -1577,44 +1693,44 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S14">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S14">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S14">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S14">
-    <cfRule type="colorScale" priority="5">
+  <conditionalFormatting sqref="S20">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S20">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S20">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S20">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>